<commit_message>
CHARMS RAS @CP2-3730 @CP2-3703 Verying participants can complete screeners, verifying that the Consent Record field Assent signed is true after minor aged 11-13 submits assent.
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario_Consent_Age_11-13.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario_Consent_Age_11-13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633D3330-10A9-9B45-A605-A7B90A437586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA7409A-B292-DE4F-B08D-0ED4E90DA688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1380" windowWidth="30240" windowHeight="17480" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17480" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenarioAge11-13" sheetId="1" r:id="rId1"/>
@@ -1098,9 +1098,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>CHARMS RAS Parent</t>
-  </si>
-  <si>
     <t>Parent</t>
   </si>
   <si>
@@ -1110,9 +1107,6 @@
     <t>What is the name of the person who may be eligible for this study? MI</t>
   </si>
   <si>
-    <t>CHARMS RAS Minor</t>
-  </si>
-  <si>
     <t>What is the name of the person who may be eligible for this study? Last</t>
   </si>
   <si>
@@ -1131,9 +1125,6 @@
     <t>What is the name of the person who may be eligible for this study?</t>
   </si>
   <si>
-    <t>CHARMS RAS Minor Test</t>
-  </si>
-  <si>
     <t>What is your relationship to the participant?</t>
   </si>
   <si>
@@ -1149,10 +1140,19 @@
     <t>Is the participant alive?</t>
   </si>
   <si>
-    <t>CHARMS RAS Parent Test</t>
-  </si>
-  <si>
     <t>consent_participant@yopmail.com</t>
+  </si>
+  <si>
+    <t>CHARMSRasMinor Test</t>
+  </si>
+  <si>
+    <t>CHARMSRasMinor</t>
+  </si>
+  <si>
+    <t>CHARMSRasParent Test</t>
+  </si>
+  <si>
+    <t>CHARMSRasParent</t>
   </si>
 </sst>
 </file>
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1611,23 +1611,23 @@
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>327</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>345</v>
@@ -1651,15 +1651,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>327</v>
@@ -1675,15 +1675,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>58</v>
@@ -1691,12 +1691,12 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B14" s="15">
         <v>41212</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>58</v>
@@ -1784,7 +1784,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1792,7 +1792,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>